<commit_message>
extra attributen ingevuld op otl_object
</commit_message>
<xml_diff>
--- a/UploadAfschermendeConstructies/analyse_afschermende_constructies.xlsx
+++ b/UploadAfschermendeConstructies/analyse_afschermende_constructies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="172">
   <si>
     <t>properties.type</t>
   </si>
@@ -1366,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F188"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2350,10 +2350,10 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E62">
-        <v>297</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2364,24 +2364,27 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E63">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="D64" t="s">
+        <v>46</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2392,27 +2395,27 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E65">
-        <v>10</v>
+        <v>252</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>77</v>
+        <v>23</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
       </c>
       <c r="E66">
-        <v>252</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2426,10 +2429,10 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2437,16 +2440,16 @@
         <v>171</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E68">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2457,13 +2460,13 @@
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D69" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="E69">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2474,27 +2477,24 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
-      </c>
-      <c r="D70" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="E70">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E71">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2502,13 +2502,13 @@
         <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2519,55 +2519,55 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D73" t="s">
+        <v>44</v>
       </c>
       <c r="E73">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="E74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>84</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>86</v>
+    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>7</v>
       </c>
       <c r="B76" t="s">
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2575,103 +2575,103 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="E77">
-        <v>116</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E78">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E80">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E81">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="F82" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E83">
-        <v>39</v>
-      </c>
-      <c r="F83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -2679,10 +2679,10 @@
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E84">
-        <v>1754</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,10 +2693,10 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E85">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,10 +2707,10 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E86">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
         <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E87">
         <v>3</v>
@@ -2735,10 +2735,10 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2749,35 +2749,23 @@
         <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E89">
-        <v>252</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>7</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
       <c r="C90" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E90">
-        <v>349</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>7</v>
-      </c>
-      <c r="B91" t="s">
-        <v>6</v>
-      </c>
       <c r="C91" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E91">
         <v>6</v>
@@ -2785,23 +2773,23 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E93">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -2809,145 +2797,145 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E95">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>100</v>
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>10</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>163</v>
+      </c>
       <c r="C97" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="E97">
         <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
       <c r="C98" t="s">
+        <v>102</v>
+      </c>
+      <c r="E98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>103</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>104</v>
+      </c>
+      <c r="E100">
         <v>11</v>
-      </c>
-      <c r="D98" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>163</v>
-      </c>
-      <c r="C99" t="s">
-        <v>101</v>
-      </c>
-      <c r="E99">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" t="s">
-        <v>102</v>
-      </c>
-      <c r="E100">
-        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E102">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="E103">
-        <v>4</v>
+        <v>77</v>
+      </c>
+      <c r="F103" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C104" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E104">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>163</v>
-      </c>
       <c r="C105" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E105">
-        <v>77</v>
-      </c>
-      <c r="F105" t="s">
-        <v>167</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E106">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C107" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E107">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E108">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C109" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C110" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E110">
         <v>2</v>
@@ -2955,15 +2943,15 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E111">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E112">
         <v>2</v>
@@ -2971,15 +2959,15 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="E113">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E114">
         <v>2</v>
@@ -2987,117 +2975,117 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C115" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C116" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E116">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E117">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>163</v>
+      </c>
       <c r="C118" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E118">
-        <v>7</v>
+        <v>62</v>
+      </c>
+      <c r="F118" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C119" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E119">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
+        <v>18</v>
+      </c>
+      <c r="E120">
         <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>163</v>
-      </c>
-      <c r="C120" t="s">
-        <v>118</v>
-      </c>
-      <c r="E120">
-        <v>62</v>
-      </c>
-      <c r="F120" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C121" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E121">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C122" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E123">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="E124">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E125">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E126">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E127">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C128" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="E128">
         <v>2</v>
@@ -3105,15 +3093,15 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C129" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E129">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E130">
         <v>2</v>
@@ -3121,118 +3109,118 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C131" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E131">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C132" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E132">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>4</v>
+      </c>
       <c r="C133" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E133">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>169</v>
+      </c>
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
       <c r="C134" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="E134">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>169</v>
+      </c>
       <c r="B135" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135" t="s">
+        <v>82</v>
+      </c>
+      <c r="E135">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C136" t="s">
+        <v>131</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C137" t="s">
+        <v>132</v>
+      </c>
+      <c r="E137">
         <v>4</v>
-      </c>
-      <c r="C135" t="s">
-        <v>130</v>
-      </c>
-      <c r="E135">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>169</v>
-      </c>
-      <c r="B136" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" t="s">
-        <v>81</v>
-      </c>
-      <c r="E136">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>169</v>
-      </c>
-      <c r="B137" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137" t="s">
-        <v>82</v>
-      </c>
-      <c r="E137">
-        <v>225</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C138" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C139" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E139">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C140" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E140">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C141" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E141">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C142" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E142">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C143" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E143">
         <v>2</v>
@@ -3240,192 +3228,201 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E144">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E145">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C146" t="s">
+        <v>141</v>
+      </c>
+      <c r="E146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>142</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
+        <v>143</v>
+      </c>
+      <c r="E148">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C146" t="s">
-        <v>139</v>
-      </c>
-      <c r="E146">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C147" t="s">
-        <v>140</v>
-      </c>
-      <c r="E147">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C148" t="s">
-        <v>141</v>
-      </c>
-      <c r="E148">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C149" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C150" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C151" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E151">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C152" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E152">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C153" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E153">
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C154" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E154">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C155" t="s">
+        <v>150</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
+        <v>80</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C157" t="s">
+        <v>151</v>
+      </c>
+      <c r="E157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C158" t="s">
+        <v>152</v>
+      </c>
+      <c r="E158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C155" t="s">
-        <v>148</v>
-      </c>
-      <c r="E155">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="156" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C156" t="s">
-        <v>149</v>
-      </c>
-      <c r="E156">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="157" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C157" t="s">
+      <c r="C159" t="s">
+        <v>153</v>
+      </c>
+      <c r="E159">
         <v>150</v>
       </c>
-      <c r="E157">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C160" t="s">
+        <v>154</v>
+      </c>
+      <c r="E160">
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C158" t="s">
-        <v>80</v>
-      </c>
-      <c r="E158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C159" t="s">
-        <v>151</v>
-      </c>
-      <c r="E159">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C160" t="s">
-        <v>152</v>
-      </c>
-      <c r="E160">
-        <v>5</v>
-      </c>
-    </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>7</v>
-      </c>
-      <c r="B161" t="s">
-        <v>4</v>
-      </c>
       <c r="C161" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E161">
-        <v>150</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C162" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E162">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C163" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E163">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C164" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E164">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>170</v>
+      </c>
+      <c r="B165" t="s">
+        <v>4</v>
+      </c>
       <c r="C165" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="E165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C166" t="s">
-        <v>158</v>
-      </c>
-      <c r="E166">
-        <v>4</v>
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E166" s="1">
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -3433,62 +3430,65 @@
         <v>170</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C167" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E167">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E168" s="1">
-        <v>114</v>
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C168" t="s">
+        <v>159</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>170</v>
-      </c>
-      <c r="B169" t="s">
-        <v>6</v>
-      </c>
       <c r="C169" t="s">
-        <v>21</v>
+        <v>160</v>
       </c>
       <c r="E169">
-        <v>2294</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C170" t="s">
-        <v>159</v>
+        <v>19</v>
       </c>
       <c r="E170">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>4</v>
+      </c>
       <c r="C171" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E171">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
       <c r="C172" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="E172">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -3496,13 +3496,13 @@
         <v>7</v>
       </c>
       <c r="B173" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -3513,10 +3513,10 @@
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E174">
-        <v>34</v>
+        <v>262</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3527,10 +3527,10 @@
         <v>6</v>
       </c>
       <c r="C175" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E175">
-        <v>63</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3541,10 +3541,10 @@
         <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E176">
-        <v>262</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -3555,10 +3555,10 @@
         <v>6</v>
       </c>
       <c r="C177" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E177">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
@@ -3569,10 +3569,10 @@
         <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E178">
-        <v>9</v>
+        <v>541</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
@@ -3583,10 +3583,10 @@
         <v>6</v>
       </c>
       <c r="C179" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E179">
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
@@ -3597,10 +3597,10 @@
         <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E180">
-        <v>541</v>
+        <v>100</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
@@ -3611,10 +3611,10 @@
         <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E181">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
@@ -3625,10 +3625,10 @@
         <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E182">
-        <v>346</v>
+        <v>143</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
@@ -3639,10 +3639,10 @@
         <v>6</v>
       </c>
       <c r="C183" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E183">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
@@ -3653,10 +3653,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E184">
-        <v>8</v>
+        <v>391</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3667,51 +3667,9 @@
         <v>6</v>
       </c>
       <c r="C185" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E185">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>7</v>
-      </c>
-      <c r="B186" t="s">
-        <v>6</v>
-      </c>
-      <c r="C186" t="s">
-        <v>70</v>
-      </c>
-      <c r="E186">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>7</v>
-      </c>
-      <c r="B187" t="s">
-        <v>6</v>
-      </c>
-      <c r="C187" t="s">
-        <v>71</v>
-      </c>
-      <c r="E187">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>7</v>
-      </c>
-      <c r="B188" t="s">
-        <v>6</v>
-      </c>
-      <c r="C188" t="s">
-        <v>72</v>
-      </c>
-      <c r="E188">
         <v>279</v>
       </c>
     </row>

</xml_diff>